<commit_message>
* in progress, several issues in paralel
</commit_message>
<xml_diff>
--- a/docs/semi-structured/LAM_metadata_20191209_JKU.xlsx
+++ b/docs/semi-structured/LAM_metadata_20191209_JKU.xlsx
@@ -20,10 +20,10 @@
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'CELEX classes'!$A$1:$N$276</definedName>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'LAM classes'!$L$1:$L$71</definedName>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'LAM properties'!$A$1:$AK$118</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'LAM properties'!$A$1:$AJ$118</definedName>
     <definedName function="false" hidden="true" localSheetId="6" name="_xlnm._FilterDatabase" vbProcedure="false">'prefixes (aux)'!$A$1:$B$52</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0" vbProcedure="false">'LAM properties'!$A$1:$AJ$108</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'LAM properties'!$A$1:$AJ$118</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'LAM properties'!$A$1:$AK$118</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -1456,7 +1456,7 @@
     <t xml:space="preserve">cdm:concept_eurovoc</t>
   </si>
   <si>
-    <t xml:space="preserve"> eurovoc:100141</t>
+    <t xml:space="preserve"> eurovoc:eurovoc</t>
   </si>
   <si>
     <r>
@@ -19879,9 +19879,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>220320</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>669960</xdr:rowOff>
+      <xdr:colOff>219960</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>445680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -19891,7 +19891,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7830720" cy="8148960"/>
+          <a:ext cx="7830360" cy="445680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -19925,8 +19925,8 @@
     <xdr:to>
       <xdr:col>27</xdr:col>
       <xdr:colOff>637560</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>2037600</xdr:rowOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>445680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -19936,7 +19936,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10041120" cy="9516600"/>
+          <a:ext cx="10040400" cy="445680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -19974,9 +19974,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>454680</xdr:colOff>
+      <xdr:colOff>454320</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>173520</xdr:rowOff>
+      <xdr:rowOff>173160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -19986,7 +19986,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="17852760" cy="4612680"/>
+          <a:ext cx="17853120" cy="4612320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -20024,13 +20024,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+  <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AK118"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
@@ -20042,18 +20042,18 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="4" min="4" style="1" width="26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="5" min="5" style="2" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="6" min="6" style="1" width="25.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="6" min="6" style="1" width="25.4"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="2" max="7" min="7" style="1" width="22.57"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="2" max="8" min="8" style="1" width="20.57"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="2" max="9" min="9" style="1" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="2" max="10" min="10" style="1" width="22.57"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="2" max="11" min="11" style="1" width="23.87"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="2" max="11" min="11" style="1" width="23.88"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="2" max="12" min="12" style="1" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="2" max="13" min="13" style="1" width="18.13"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="2" max="13" min="13" style="1" width="18.12"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="2" max="14" min="14" style="1" width="17.71"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="2" max="15" min="15" style="1" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="2" max="16" min="16" style="1" width="32.57"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="2" max="17" min="17" style="1" width="17.41"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="2" max="17" min="17" style="1" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="2" max="18" min="18" style="1" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="2" max="19" min="19" style="1" width="22.57"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="2" max="20" min="20" style="1" width="13.7"/>
@@ -20191,7 +20191,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B2)</f>
         <v>lamd:md_CODE</v>
@@ -20234,7 +20234,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B3)</f>
         <v>lamd:md_LABEL</v>
@@ -20277,7 +20277,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="30" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B4)</f>
         <v>lamd:md_KEYWORD</v>
@@ -20323,7 +20323,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B5)</f>
         <v>lamd:md_EXAMPLE_EN</v>
@@ -20369,7 +20369,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B6)</f>
         <v>lamd:md_EXAMPLE_FR</v>
@@ -20415,7 +20415,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="30" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B7)</f>
         <v>lamd:md_COMMENT</v>
@@ -20461,7 +20461,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="30" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B8)</f>
         <v>lamd:md_EXAMPLE_CELEX</v>
@@ -20507,7 +20507,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="24" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B9)</f>
         <v>lamd:md_CDM_CLASS</v>
@@ -20553,7 +20553,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="186" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="186" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B10)</f>
         <v>lamd:md_AU</v>
@@ -20620,7 +20620,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="90" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B11)</f>
         <v>lamd:md_FM</v>
@@ -20685,7 +20685,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B12)</f>
         <v>lamd:md_DT_CORR</v>
@@ -20746,7 +20746,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="30" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B13)</f>
         <v>lamd:md_DN_CLASS</v>
@@ -20789,7 +20789,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="210.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="210.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B14)</f>
         <v>lamd:md_DN</v>
@@ -20914,7 +20914,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="360" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="360" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B16)</f>
         <v>lamd:md_CT</v>
@@ -20975,7 +20975,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="409.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B17)</f>
         <v>lamd:md_CC</v>
@@ -21039,7 +21039,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="90" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B18)</f>
         <v>lamd:md_RJ_NEW</v>
@@ -21100,7 +21100,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="167.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="167.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B19)</f>
         <v>lamd:md_DD</v>
@@ -21170,7 +21170,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="156" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="156" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B20)</f>
         <v>lamd:md_IF</v>
@@ -21243,7 +21243,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="156" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="156" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B21)</f>
         <v>lamd:md_EV</v>
@@ -21313,7 +21313,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="148.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="148.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B22)</f>
         <v>lamd:md_NF</v>
@@ -21380,7 +21380,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="105" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B23)</f>
         <v>lamd:md_TP</v>
@@ -21449,7 +21449,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B24)</f>
         <v>lamd:md_SG</v>
@@ -21515,7 +21515,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="60" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B25)</f>
         <v>lamd:md_VO</v>
@@ -21576,7 +21576,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="90" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B26)</f>
         <v>lamd:md_DB</v>
@@ -21639,7 +21639,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="105" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B27)</f>
         <v>lamd:md_LO</v>
@@ -21699,7 +21699,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="270" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="270" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B28)</f>
         <v>lamd:md_DH</v>
@@ -21765,7 +21765,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="23.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B29)</f>
         <v>lamd:md_DL</v>
@@ -21829,7 +21829,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B30)</f>
         <v>lamd:md_RP</v>
@@ -21899,7 +21899,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="409.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B31)</f>
         <v>lamd:md_VV</v>
@@ -21962,7 +21962,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="409.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B32)</f>
         <v>lamd:md_REP</v>
@@ -22028,7 +22028,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="210" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="210" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B33)</f>
         <v>lamd:md_RS</v>
@@ -22094,7 +22094,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="135" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="135" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B34)</f>
         <v>lamd:md_AS</v>
@@ -22160,7 +22160,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B35)</f>
         <v>lamd:md_AF</v>
@@ -22221,7 +22221,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="409.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B36)</f>
         <v>lamd:md_MI</v>
@@ -22285,7 +22285,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="105" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B37)</f>
         <v>lamd:md_LG</v>
@@ -22348,7 +22348,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="60" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B38)</f>
         <v>lamd:md_RI</v>
@@ -22405,7 +22405,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="60" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B39)</f>
         <v>lamd:md_DP</v>
@@ -22471,7 +22471,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="375" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="375" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B40)</f>
         <v>lamd:md_AD</v>
@@ -22537,7 +22537,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B41)</f>
         <v>lamd:md_LF</v>
@@ -22597,7 +22597,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="210" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="210" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B42)</f>
         <v>lamd:md_REPPORTEUR</v>
@@ -22663,7 +22663,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B43)</f>
         <v>lamd:md_IC</v>
@@ -22726,7 +22726,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="240" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="240" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B44)</f>
         <v>lamd:md_CM</v>
@@ -22789,7 +22789,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="135" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="135" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B45)</f>
         <v>lamd:md_NS</v>
@@ -22852,7 +22852,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B46)</f>
         <v>lamd:md_TT</v>
@@ -22918,7 +22918,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="228" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="228" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B47)</f>
         <v>lamd:md_LB</v>
@@ -22999,7 +22999,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="135" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="135" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B48)</f>
         <v>lamd:md_AMENDMENT</v>
@@ -23092,7 +23092,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="228" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="228" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B49)</f>
         <v>lamd:md_ADDITION</v>
@@ -23188,7 +23188,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="180" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="180" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B50)</f>
         <v>lamd:md_REPEAL</v>
@@ -23281,7 +23281,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="195" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="195" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B51)</f>
         <v>lamd:md_REPEAL_IMP</v>
@@ -23374,7 +23374,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="180" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="180" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B52)</f>
         <v>lamd:md_ADOPTION</v>
@@ -23467,7 +23467,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="216" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="216" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B53)</f>
         <v>lamd:md_ADOPTION_PAR</v>
@@ -23560,7 +23560,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="204" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="204" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B54)</f>
         <v>lamd:md_APPLICABILITY_EXT</v>
@@ -23653,7 +23653,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="195" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="195" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B55)</f>
         <v>lamd:md_COMPLETION</v>
@@ -23749,7 +23749,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="192" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="192" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B56)</f>
         <v>lamd:md_VALIDITY_EXT</v>
@@ -23845,7 +23845,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="180" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="180" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B57)</f>
         <v>lamd:md_REPLACEMENT</v>
@@ -23941,7 +23941,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="168" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="168" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B58)</f>
         <v>lamd:md_CORRIGENDUM</v>
@@ -24034,7 +24034,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="192" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="192" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B59)</f>
         <v>lamd:md_OBSOLETE</v>
@@ -24127,7 +24127,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="252" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="252" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B60)</f>
         <v>lamd:md_DEROGATION</v>
@@ -24223,7 +24223,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="60" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B61)</f>
         <v>lamd:md_CONFIRMATION</v>
@@ -24316,7 +24316,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B62)</f>
         <v>lamd:md_QUESTION_SIMILAR</v>
@@ -24409,7 +24409,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="135" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="135" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B63)</f>
         <v>lamd:md_INTERPRETATION</v>
@@ -24499,7 +24499,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="90" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B64)</f>
         <v>lamd:md_IMPLEMENTATION</v>
@@ -24592,7 +24592,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B65)</f>
         <v>lamd:md_REESTAB</v>
@@ -24685,7 +24685,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B66)</f>
         <v>lamd:md_SUSPEND</v>
@@ -24775,7 +24775,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B67)</f>
         <v>lamd:md_SUSPEND_PAR</v>
@@ -24868,7 +24868,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="228" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="228" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B68)</f>
         <v>lamd:md_APPLICABILITY_DEF</v>
@@ -24961,7 +24961,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B69)</f>
         <v>lamd:md_INCORPORATION</v>
@@ -25054,7 +25054,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B70)</f>
         <v>lamd:md_REFER_PAR</v>
@@ -25144,7 +25144,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="216" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="216" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B71)</f>
         <v>lamd:md_QUESTION_RELATED</v>
@@ -25237,7 +25237,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="60" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B72)</f>
         <v>lamd:md_OPINION_EP</v>
@@ -25328,7 +25328,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="60" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B73)</f>
         <v>lamd:md_OPINION_COR</v>
@@ -25418,7 +25418,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="60" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B74)</f>
         <v>lamd:md_OPINION_EESC</v>
@@ -25508,7 +25508,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B75)</f>
         <v>lamd:md_INFLUENCE</v>
@@ -25598,7 +25598,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="135" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="135" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B76)</f>
         <v>lamd:md_AMENDMENT_PRO</v>
@@ -25688,7 +25688,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="288" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="288" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B77)</f>
         <v>lamd:md_CI</v>
@@ -25760,7 +25760,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="409.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B78)</f>
         <v>lamd:md_RELATION</v>
@@ -25832,7 +25832,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="192" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="192" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B79)</f>
         <v>lamd:md_ASSOCIATION</v>
@@ -25904,7 +25904,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B80)</f>
         <v>lamd:md_PROC</v>
@@ -25955,7 +25955,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="165" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="165" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B81)</f>
         <v>lamd:md_AP</v>
@@ -26015,7 +26015,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="165" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="165" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B82)</f>
         <v>lamd:md_DF</v>
@@ -26075,7 +26075,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B83)</f>
         <v>lamd:md_PR</v>
@@ -26135,7 +26135,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B84)</f>
         <v>lamd:md_NA</v>
@@ -26192,7 +26192,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="60" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B85)</f>
         <v>lamd:md_ANNULMENT_REQ</v>
@@ -26279,7 +26279,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="60" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B86)</f>
         <v>lamd:md_FAILURE_REQ</v>
@@ -26366,7 +26366,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="60" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B87)</f>
         <v>lamd:md_INAPPLICAB_REQ</v>
@@ -26453,7 +26453,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="60" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B88)</f>
         <v>lamd:md_ANULMENT_PARTIAL_REQ</v>
@@ -26540,7 +26540,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="60" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B89)</f>
         <v>lamd:md_REVIEW_REQ</v>
@@ -26627,7 +26627,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B90)</f>
         <v>lamd:md_PRELIMINARY_REQ</v>
@@ -26714,7 +26714,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="60" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B91)</f>
         <v>lamd:md_COMMUNIC_REQ</v>
@@ -26801,7 +26801,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="60" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B92)</f>
         <v>lamd:md_OPINION_REQ</v>
@@ -26888,7 +26888,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="150" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B93)</f>
         <v>lamd:md_ANN_COD</v>
@@ -26951,7 +26951,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="60" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B94)</f>
         <v>lamd:md_ANN_TOD</v>
@@ -27014,7 +27014,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="60" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B95)</f>
         <v>lamd:md_ANN_CLB</v>
@@ -27074,7 +27074,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B96)</f>
         <v>lamd:md_ANN_ART</v>
@@ -27128,7 +27128,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="30" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B97)</f>
         <v>lamd:md_ANN_PAR</v>
@@ -27182,7 +27182,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="30" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B98)</f>
         <v>lamd:md_ANN_SUB</v>
@@ -27236,7 +27236,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="60" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B99)</f>
         <v>lamd:md_ANN_TLT</v>
@@ -27293,7 +27293,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="30" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B100)</f>
         <v>lamd:md_ANN_RL2</v>
@@ -27350,7 +27350,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B101)</f>
         <v>lamd:md_ANN_MDL</v>
@@ -27410,7 +27410,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B102)</f>
         <v>lamd:md_ANN_MSL</v>
@@ -27470,7 +27470,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="60" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B103)</f>
         <v>lamd:md_ANN_SOV</v>
@@ -27521,7 +27521,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="30" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B104)</f>
         <v>lamd:md_ANN_EOV</v>
@@ -27572,7 +27572,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="30" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B105)</f>
         <v>lamd:md_ANN_LVL</v>
@@ -27629,7 +27629,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="30" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B106)</f>
         <v>lamd:md_ANN_FCS</v>
@@ -27686,7 +27686,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="30" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B107)</f>
         <v>lamd:md_ANN_FCT</v>
@@ -27728,7 +27728,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="195" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="195" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B108)</f>
         <v>lamd:md_DTS</v>
@@ -27767,7 +27767,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="60" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B109)</f>
         <v>lamd:md_DTT</v>
@@ -27803,7 +27803,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="165" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="165" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B110)</f>
         <v>lamd:md_DTA</v>
@@ -27842,7 +27842,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="135" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="135" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B111)</f>
         <v>lamd:md_DTN</v>
@@ -27881,7 +27881,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="90" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B112)</f>
         <v>lamd:md_OJ_ID</v>
@@ -27914,7 +27914,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="30" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B113)</f>
         <v>lamd:md_ELI</v>
@@ -27935,7 +27935,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="30" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B114)</f>
         <v>lamd:md_ECLI</v>
@@ -27956,7 +27956,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B115)</f>
         <v>lamd:md_PARENT</v>
@@ -27977,7 +27977,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B116)</f>
         <v>lamd:md_ORDER</v>
@@ -28001,7 +28001,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B117)</f>
         <v>lamd:md_DESCRIPTION</v>
@@ -28022,7 +28022,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="30" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="str">
         <f aca="false">CONCATENATE("lamd:md_",B118)</f>
         <v>lamd:md_CLASSIFICATION</v>
@@ -28044,7 +28044,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AK118"/>
+  <autoFilter ref="A1:AJ118">
+    <filterColumn colId="5">
+      <customFilters and="true">
+        <customFilter operator="equal" val=" eurovoc:100141"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -28587,7 +28593,7 @@
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="23" width="40.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="23" width="40.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="23" width="67.71"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="5" min="5" style="23" width="67.71"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="6" min="6" style="23" width="80.14"/>
@@ -36686,7 +36692,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16"/>
@@ -37256,13 +37262,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="27.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="27.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="17.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="40.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="40.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="6" min="6" style="2" width="93.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="7" min="7" style="2" width="63.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="7" min="7" style="2" width="63.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="8" min="8" style="2" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="9" min="9" style="2" width="22.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="10" min="10" style="2" width="22.57"/>

</xml_diff>